<commit_message>
final touches for the project 4 presentation
</commit_message>
<xml_diff>
--- a/Template-SEO-audit.xlsx
+++ b/Template-SEO-audit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
   <si>
     <t>Category</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>(SEO or Accessibility?)</t>
-  </si>
-  <si>
     <t>Image natural dimensions should be proportional to the display size and the pixel ratio to maximize image clarity.</t>
   </si>
   <si>
@@ -142,30 +139,6 @@
     <t>https://catswhocode.com/how-to-make-a-responsive-website/</t>
   </si>
   <si>
-    <t>Image elements do not have explicit width and height</t>
-  </si>
-  <si>
-    <t>Set an explicit width and height on image elements to reduce layout shifts and improve CLS</t>
-  </si>
-  <si>
-    <t>Adding the right width and height to image elements will help reduce layout shifts and improve page loading</t>
-  </si>
-  <si>
-    <t>https://web.dev/optimize-cls/?utm_source=lighthouse&amp;utm_medium=devtools#images-without-dimensions</t>
-  </si>
-  <si>
-    <t>Enable text compression</t>
-  </si>
-  <si>
-    <t>Text-based resources should be served with compression (gzip, deflate or brotli) to minimize total network bytes</t>
-  </si>
-  <si>
-    <t>https://web.dev/uses-text-compression/?utm_source=lighthouse&amp;utm_medium=devtools</t>
-  </si>
-  <si>
-    <t>If the original size of a response is less than 1.4KiB, or if the potential compression savings is less than 10% of the original size, then Lighthouse does not flag that response in the results.</t>
-  </si>
-  <si>
     <t>Remove unused CSS</t>
   </si>
   <si>
@@ -178,30 +151,9 @@
     <t>The Opportunities section of your Lighthouse report lists all stylesheets with unused CSS with a potential savings of 2 KiB or more</t>
   </si>
   <si>
-    <t>Ensure text remains visible during webfont load</t>
-  </si>
-  <si>
     <t>Links do not have a discernible name</t>
   </si>
   <si>
-    <t>Avoid enormous network payloads </t>
-  </si>
-  <si>
-    <t>Large network payloads cost users real money and are highly correlated with long load times.</t>
-  </si>
-  <si>
-    <t>https://web.dev/total-byte-weight/?utm_source=lighthouse&amp;utm_medium=devtools</t>
-  </si>
-  <si>
-    <t>Leverage the font-display CSS feature to ensure text is user-visible while webfonts are loading.</t>
-  </si>
-  <si>
-    <t>https://web.dev/font-display/?utm_source=lighthouse&amp;utm_medium=devtools</t>
-  </si>
-  <si>
-    <t>The easiest way to avoid showing invisible text while custom fonts load is to temporarily show a system font.</t>
-  </si>
-  <si>
     <t>https://developers.google.com/web/fundamentals/accessibility/how-to-review?utm_source=lighthouse&amp;utm_medium=devtools</t>
   </si>
   <si>
@@ -209,42 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve">Link text (and alternate text for images, when used as links) that is discernible, unique, and focusable improves the navigation experience for screen reader users. </t>
-  </si>
-  <si>
-    <t>Includes front-end JavaScript libraries with known security vulnerabilities </t>
-  </si>
-  <si>
-    <t>Some third-party scripts may contain known security vulnerabilities that are easily identified and exploited by attackers.</t>
-  </si>
-  <si>
-    <t>https://web.dev/no-vulnerable-libraries/?utm_source=lighthouse&amp;utm_medium=devtools</t>
-  </si>
-  <si>
-    <t>Intruders have automated web crawlers that can scan your site for known security vulnerabilities. When the web crawler detects a vulnerability, it alerts the intruder. From there, the intruder just needs to figure out how to exploit the vulnerability on your site.</t>
-  </si>
-  <si>
-    <r>
-      <t>Reducing the total size of your page's network requests is good for your users' experience on your site </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>and</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t> their wallets.</t>
-    </r>
   </si>
   <si>
     <r>
@@ -326,12 +242,48 @@
   <si>
     <t>Serves images with low resolution, serves images in png and jpg formats</t>
   </si>
+  <si>
+    <t>The unused CSS has been removed in order to improve performance</t>
+  </si>
+  <si>
+    <t>Changed the alternative description to make it relevant to each picture</t>
+  </si>
+  <si>
+    <t>Multiple H1 tags on the website</t>
+  </si>
+  <si>
+    <t>There should be only one H1 tag on the website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do not use multiple H1 tags on the website </t>
+  </si>
+  <si>
+    <t>I have changed the H1 tags to H2 tags leaving only one main relevant title</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/en/courses/3594061-drive-traffic-to-your-website-with-search-engine-optimization-seo/5838156-optimize-the-content-of-your-web-pages</t>
+  </si>
+  <si>
+    <t>Missing structural html elements and aria landmarks</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/en/courses/6663451-make-your-web-content-accessible/6913058-annotate-mock-ups-and-wireframes-with-accessibility-information</t>
+  </si>
+  <si>
+    <t>To make the page easier to navigate for assistive technology users, you should define the main regions of your page using either structural HTML elements, ARIA landmark roles, or both. It will allow users to quickly understand how the page is organized and what regions are available. It will also help them move around the content quickly and efficiently.</t>
+  </si>
+  <si>
+    <t>Use structural html elements in order to make it easy to navigate the website</t>
+  </si>
+  <si>
+    <t>Do not use only divs instead of all structural html elements</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -351,13 +303,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -466,55 +411,38 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -522,6 +450,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -732,404 +670,340 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="7" customWidth="1"/>
-    <col min="2" max="4" width="21.33203125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" style="9" customWidth="1"/>
-    <col min="7" max="26" width="10.5546875" style="7" customWidth="1"/>
-    <col min="27" max="16384" width="11.21875" style="7"/>
+    <col min="1" max="1" width="21.33203125" style="6" customWidth="1"/>
+    <col min="2" max="4" width="21.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="21.33203125" style="7" customWidth="1"/>
+    <col min="7" max="26" width="10.5546875" style="6" customWidth="1"/>
+    <col min="27" max="16384" width="11.21875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:26" ht="112.5">
+      <c r="A2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8" t="b">
-        <v>0</v>
+      <c r="D2" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="112.5">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:26" ht="93.75">
+      <c r="A3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="225">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="131.25">
+      <c r="A5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="73.5" customHeight="1">
+      <c r="A6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="19" t="s">
+      <c r="B6" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="93.75">
+      <c r="A7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="69" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="112.5">
+      <c r="A9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="131.25">
+      <c r="A10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="150">
+      <c r="A11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="168.75">
+      <c r="A12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="82.5">
+      <c r="A13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="226.5">
+      <c r="A14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="D14" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:26" ht="93.75">
-      <c r="A4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="225">
-      <c r="A5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="131.25">
-      <c r="A6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="73.5" customHeight="1">
-      <c r="A7" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="93.75">
-      <c r="A8" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="69" customHeight="1">
-      <c r="A9" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="112.5">
-      <c r="A10" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="131.25">
-      <c r="A11" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="112.5">
-      <c r="A12" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="8" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="168.75">
-      <c r="A13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="150">
-      <c r="A14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="112.5">
-      <c r="A15" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="93.75">
-      <c r="A16" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="168.75">
-      <c r="A17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E17" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="243.75">
-      <c r="A18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E18" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="30" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="31" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="32" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
+    <row r="21" ht="15.75" customHeight="1"/>
+    <row r="22" ht="15.75" customHeight="1"/>
+    <row r="23" ht="15.75" customHeight="1"/>
+    <row r="24" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1"/>
+    <row r="26" ht="15.75" customHeight="1"/>
+    <row r="27" ht="15.75" customHeight="1"/>
+    <row r="28" ht="15.75" customHeight="1"/>
+    <row r="29" ht="15.75" customHeight="1"/>
+    <row r="30" ht="15.75" customHeight="1"/>
+    <row r="31" ht="15.75" customHeight="1"/>
+    <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2088,18 +1962,14 @@
     <row r="988" ht="15.75" customHeight="1"/>
     <row r="989" ht="15.75" customHeight="1"/>
     <row r="990" ht="15.75" customHeight="1"/>
-    <row r="991" ht="15.75" customHeight="1"/>
-    <row r="992" ht="15.75" customHeight="1"/>
-    <row r="993" ht="15.75" customHeight="1"/>
-    <row r="994" ht="15.75" customHeight="1"/>
-    <row r="995" ht="15.75" customHeight="1"/>
-    <row r="996" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F5" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId1"/>
+    <hyperlink ref="F13" r:id="rId2" display="https://openclassrooms.com/en/courses/3594061-drive-traffic-to-your-website-with-search-engine-optimization-seo/5838156-optimize-the-content-of-your-web-pages?fbclid=IwAR30r1q6KHOZbIyI7LjQcKleRjF5dy7RVdLO8RBDazT0m0wbsedfJ9DZPv0"/>
+    <hyperlink ref="F14" r:id="rId3" display="https://openclassrooms.com/en/courses/6663451-make-your-web-content-accessible/6913058-annotate-mock-ups-and-wireframes-with-accessibility-information?fbclid=IwAR00YlOdH1oqX8LsnYyhFyipsXVYcw1Hl5dAPfsbgrcQsZ6VDJlOdAmVvUY"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId2"/>
+  <pageSetup orientation="landscape" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2115,10 +1985,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="22.5">
       <c r="A1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>70</v>
+        <v>48</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>